<commit_message>
Just update commit before travel
Update to bring everything to same place before travelling.
</commit_message>
<xml_diff>
--- a/Documents/ChunkUpdateMath.xlsx
+++ b/Documents/ChunkUpdateMath.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualStudioProjects\PixelProject\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C14F46-497B-4440-AD25-B3571964B447}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13526A7B-CA80-4843-B520-29798D446D32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31305" yWindow="7140" windowWidth="21600" windowHeight="11475" activeTab="3" xr2:uid="{11E5D31D-36D7-45CF-BBA8-6E265D1131AF}"/>
+    <workbookView xWindow="40740" yWindow="6570" windowWidth="21600" windowHeight="11475" activeTab="3" xr2:uid="{11E5D31D-36D7-45CF-BBA8-6E265D1131AF}"/>
   </bookViews>
   <sheets>
     <sheet name="ChunkUpdate" sheetId="1" r:id="rId1"/>
@@ -283,7 +283,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -434,6 +434,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5732,8 +5744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D61EA23-8960-4D35-B73F-6BF8BB0B9F26}">
   <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5750,22 +5762,54 @@
       <c r="A1" s="33"/>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
+      <c r="D1" s="60">
+        <v>0</v>
+      </c>
+      <c r="E1" s="60">
+        <v>1</v>
+      </c>
+      <c r="F1" s="60">
+        <v>2</v>
+      </c>
+      <c r="G1" s="60">
+        <v>3</v>
+      </c>
+      <c r="H1" s="60">
+        <v>4</v>
+      </c>
+      <c r="I1" s="60">
+        <v>5</v>
+      </c>
+      <c r="J1" s="60">
+        <v>6</v>
+      </c>
+      <c r="K1" s="60">
+        <v>7</v>
+      </c>
+      <c r="L1" s="60">
+        <v>8</v>
+      </c>
+      <c r="M1" s="60">
+        <v>9</v>
+      </c>
+      <c r="N1" s="60">
+        <v>10</v>
+      </c>
+      <c r="O1" s="60">
+        <v>11</v>
+      </c>
+      <c r="P1" s="60">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="60">
+        <v>13</v>
+      </c>
+      <c r="R1" s="60">
+        <v>14</v>
+      </c>
+      <c r="S1" s="60">
+        <v>15</v>
+      </c>
       <c r="T1" s="34"/>
       <c r="U1" s="34"/>
       <c r="V1" s="35"/>
@@ -5857,12 +5901,13 @@
         <v>16</v>
       </c>
       <c r="Y3" s="42">
-        <f>SUM(17+16)</f>
-        <v>33</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
+      <c r="A4" s="61">
+        <v>0</v>
+      </c>
       <c r="B4" s="37"/>
       <c r="C4" s="53">
         <v>15</v>
@@ -5919,7 +5964,9 @@
         <v>0</v>
       </c>
       <c r="U4" s="37"/>
-      <c r="V4" s="38"/>
+      <c r="V4" s="62">
+        <v>15</v>
+      </c>
       <c r="X4" s="42" t="s">
         <v>17</v>
       </c>
@@ -5928,7 +5975,9 @@
       </c>
     </row>
     <row r="5" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
+      <c r="A5" s="61">
+        <v>1</v>
+      </c>
       <c r="B5" s="37"/>
       <c r="C5" s="54">
         <v>31</v>
@@ -5985,7 +6034,9 @@
         <v>16</v>
       </c>
       <c r="U5" s="37"/>
-      <c r="V5" s="38"/>
+      <c r="V5" s="62">
+        <v>14</v>
+      </c>
       <c r="X5" s="42" t="s">
         <v>18</v>
       </c>
@@ -5994,7 +6045,9 @@
       </c>
     </row>
     <row r="6" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
+      <c r="A6" s="61">
+        <v>2</v>
+      </c>
       <c r="B6" s="37"/>
       <c r="C6" s="54">
         <v>47</v>
@@ -6051,10 +6104,14 @@
         <v>32</v>
       </c>
       <c r="U6" s="37"/>
-      <c r="V6" s="38"/>
+      <c r="V6" s="62">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
+      <c r="A7" s="61">
+        <v>3</v>
+      </c>
       <c r="B7" s="37"/>
       <c r="C7" s="54">
         <v>63</v>
@@ -6111,14 +6168,18 @@
         <v>48</v>
       </c>
       <c r="U7" s="37"/>
-      <c r="V7" s="38"/>
+      <c r="V7" s="62">
+        <v>12</v>
+      </c>
       <c r="X7" s="42">
         <f>MOD(R13,Y4)</f>
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
+      <c r="A8" s="61">
+        <v>4</v>
+      </c>
       <c r="B8" s="37"/>
       <c r="C8" s="54">
         <v>79</v>
@@ -6175,10 +6236,14 @@
         <v>64</v>
       </c>
       <c r="U8" s="37"/>
-      <c r="V8" s="38"/>
+      <c r="V8" s="62">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
+      <c r="A9" s="61">
+        <v>5</v>
+      </c>
       <c r="B9" s="37"/>
       <c r="C9" s="54">
         <v>95</v>
@@ -6235,10 +6300,18 @@
         <v>80</v>
       </c>
       <c r="U9" s="37"/>
-      <c r="V9" s="38"/>
+      <c r="V9" s="62">
+        <v>10</v>
+      </c>
+      <c r="X9" s="42">
+        <f>SUM(Y4-I4)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="36"/>
+      <c r="A10" s="61">
+        <v>6</v>
+      </c>
       <c r="B10" s="37"/>
       <c r="C10" s="54">
         <v>111</v>
@@ -6295,10 +6368,14 @@
         <v>96</v>
       </c>
       <c r="U10" s="37"/>
-      <c r="V10" s="38"/>
+      <c r="V10" s="62">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="36"/>
+      <c r="A11" s="61">
+        <v>7</v>
+      </c>
       <c r="B11" s="37"/>
       <c r="C11" s="54">
         <v>127</v>
@@ -6355,10 +6432,14 @@
         <v>112</v>
       </c>
       <c r="U11" s="37"/>
-      <c r="V11" s="38"/>
+      <c r="V11" s="62">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="36"/>
+      <c r="A12" s="61">
+        <v>8</v>
+      </c>
       <c r="B12" s="37"/>
       <c r="C12" s="54">
         <v>143</v>
@@ -6415,10 +6496,14 @@
         <v>128</v>
       </c>
       <c r="U12" s="37"/>
-      <c r="V12" s="38"/>
+      <c r="V12" s="62">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
+      <c r="A13" s="61">
+        <v>9</v>
+      </c>
       <c r="B13" s="37"/>
       <c r="C13" s="54">
         <v>159</v>
@@ -6475,10 +6560,14 @@
         <v>144</v>
       </c>
       <c r="U13" s="37"/>
-      <c r="V13" s="38"/>
+      <c r="V13" s="62">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
+      <c r="A14" s="61">
+        <v>10</v>
+      </c>
       <c r="B14" s="37"/>
       <c r="C14" s="54">
         <v>175</v>
@@ -6535,10 +6624,14 @@
         <v>160</v>
       </c>
       <c r="U14" s="37"/>
-      <c r="V14" s="38"/>
+      <c r="V14" s="62">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="36"/>
+      <c r="A15" s="61">
+        <v>11</v>
+      </c>
       <c r="B15" s="37"/>
       <c r="C15" s="54">
         <v>191</v>
@@ -6595,10 +6688,14 @@
         <v>176</v>
       </c>
       <c r="U15" s="37"/>
-      <c r="V15" s="38"/>
+      <c r="V15" s="62">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
+      <c r="A16" s="61">
+        <v>12</v>
+      </c>
       <c r="B16" s="37"/>
       <c r="C16" s="54">
         <v>207</v>
@@ -6655,10 +6752,14 @@
         <v>192</v>
       </c>
       <c r="U16" s="37"/>
-      <c r="V16" s="38"/>
+      <c r="V16" s="62">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
+      <c r="A17" s="61">
+        <v>13</v>
+      </c>
       <c r="B17" s="37"/>
       <c r="C17" s="54">
         <v>223</v>
@@ -6715,10 +6816,14 @@
         <v>208</v>
       </c>
       <c r="U17" s="37"/>
-      <c r="V17" s="38"/>
+      <c r="V17" s="62">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="36"/>
+      <c r="A18" s="61">
+        <v>14</v>
+      </c>
       <c r="B18" s="37"/>
       <c r="C18" s="54">
         <v>239</v>
@@ -6775,10 +6880,14 @@
         <v>224</v>
       </c>
       <c r="U18" s="37"/>
-      <c r="V18" s="38"/>
+      <c r="V18" s="62">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:22" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="36"/>
+      <c r="A19" s="61">
+        <v>15</v>
+      </c>
       <c r="B19" s="37"/>
       <c r="C19" s="52">
         <v>255</v>
@@ -6835,7 +6944,9 @@
         <v>240</v>
       </c>
       <c r="U19" s="37"/>
-      <c r="V19" s="38"/>
+      <c r="V19" s="62">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="36"/>
@@ -6925,25 +7036,54 @@
       <c r="A22" s="39"/>
       <c r="B22" s="40"/>
       <c r="C22" s="40"/>
-      <c r="D22" s="40">
-        <f>SUM(256-16)</f>
-        <v>240</v>
-      </c>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40"/>
-      <c r="M22" s="40"/>
-      <c r="N22" s="40"/>
-      <c r="O22" s="40"/>
-      <c r="P22" s="40"/>
-      <c r="Q22" s="40"/>
-      <c r="R22" s="40"/>
-      <c r="S22" s="40"/>
+      <c r="D22" s="63">
+        <v>15</v>
+      </c>
+      <c r="E22" s="63">
+        <v>14</v>
+      </c>
+      <c r="F22" s="63">
+        <v>13</v>
+      </c>
+      <c r="G22" s="63">
+        <v>12</v>
+      </c>
+      <c r="H22" s="63">
+        <v>11</v>
+      </c>
+      <c r="I22" s="63">
+        <v>10</v>
+      </c>
+      <c r="J22" s="63">
+        <v>9</v>
+      </c>
+      <c r="K22" s="63">
+        <v>8</v>
+      </c>
+      <c r="L22" s="63">
+        <v>7</v>
+      </c>
+      <c r="M22" s="63">
+        <v>6</v>
+      </c>
+      <c r="N22" s="63">
+        <v>5</v>
+      </c>
+      <c r="O22" s="63">
+        <v>4</v>
+      </c>
+      <c r="P22" s="63">
+        <v>3</v>
+      </c>
+      <c r="Q22" s="63">
+        <v>2</v>
+      </c>
+      <c r="R22" s="63">
+        <v>1</v>
+      </c>
+      <c r="S22" s="63">
+        <v>0</v>
+      </c>
       <c r="T22" s="40"/>
       <c r="U22" s="40"/>
       <c r="V22" s="41"/>

</xml_diff>